<commit_message>
Update Supporting Information S4.1 – Exogenous Data for Nowcasting.xlsx
</commit_message>
<xml_diff>
--- a/Supporting Information S4.1 – Exogenous Data for Nowcasting.xlsx
+++ b/Supporting Information S4.1 – Exogenous Data for Nowcasting.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ee21ap\Documents\GitHub\Code-and-Supporting-Files---AP-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36ADD8B0-9152-4E78-9CD7-F517B090A59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F8203B-68E6-43FD-AEB2-D40402B41980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{AAD8422F-E34F-4AB5-A94F-E15E5DC81DBD}"/>
+    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{AAD8422F-E34F-4AB5-A94F-E15E5DC81DBD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="GDP" sheetId="2" r:id="rId2"/>
-    <sheet name="Imports" sheetId="3" r:id="rId3"/>
-    <sheet name="Exports" sheetId="4" r:id="rId4"/>
-    <sheet name="Deflators" sheetId="5" r:id="rId5"/>
-    <sheet name="GDP_Contributions" sheetId="6" r:id="rId6"/>
+    <sheet name="GDP" sheetId="2" r:id="rId1"/>
+    <sheet name="Imports" sheetId="3" r:id="rId2"/>
+    <sheet name="Exports" sheetId="4" r:id="rId3"/>
+    <sheet name="Deflators" sheetId="5" r:id="rId4"/>
+    <sheet name="GDP_Contributions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1097,22 +1096,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C11E676-7325-42EC-8191-738F82929B86}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02996270-F963-47EF-B37F-DD194A666408}">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -2119,7 +2106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7D6A88-4633-4C00-8049-BAB182BD7441}">
   <dimension ref="A1:AA12"/>
   <sheetViews>
@@ -3130,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD8A0DB-EEAC-484F-BBD4-45EE11F3C4DE}">
   <dimension ref="A1:AA12"/>
   <sheetViews>
@@ -4141,7 +4128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2B2C68-CEFE-4E9D-9449-52495EF61FA6}">
   <dimension ref="A1:DI12"/>
   <sheetViews>
@@ -8245,11 +8232,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE6ACB5-FC6E-430C-ACB7-436AEEEA3165}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>

</xml_diff>